<commit_message>
(feature/Test):add method to get name school, detail accocunt
</commit_message>
<xml_diff>
--- a/server/Uploads/classes.xlsx
+++ b/server/Uploads/classes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenhu\OneDrive\Máy tính\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CFF751-AA0C-4CA2-9B5A-4E294B30EF16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1CB777-1A29-4D63-A43B-BBFB6C39DE51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{4055AE8D-10FB-4500-B233-61A215BE8418}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{4055AE8D-10FB-4500-B233-61A215BE8418}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -530,7 +530,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,7 +584,7 @@
         <v>29</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -608,7 +608,7 @@
         <v>30</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -632,7 +632,7 @@
         <v>31</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -656,7 +656,7 @@
         <v>32</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -680,7 +680,7 @@
         <v>33</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -704,7 +704,7 @@
         <v>34</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -728,7 +728,7 @@
         <v>35</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -752,7 +752,7 @@
         <v>36</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -776,7 +776,7 @@
         <v>37</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -800,7 +800,7 @@
         <v>38</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -824,7 +824,7 @@
         <v>39</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -848,7 +848,7 @@
         <v>40</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -872,7 +872,7 @@
         <v>41</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -896,7 +896,7 @@
         <v>42</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -920,7 +920,7 @@
         <v>43</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -944,7 +944,7 @@
         <v>44</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -968,7 +968,7 @@
         <v>45</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -992,7 +992,7 @@
         <v>46</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1016,7 +1016,7 @@
         <v>47</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1040,7 +1040,7 @@
         <v>48</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1064,7 +1064,7 @@
         <v>49</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -1088,7 +1088,7 @@
         <v>50</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1112,7 +1112,7 @@
         <v>51</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1136,7 +1136,7 @@
         <v>52</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1160,7 +1160,7 @@
         <v>53</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1184,7 +1184,7 @@
         <v>54</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -1208,7 +1208,7 @@
         <v>55</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -1232,7 +1232,7 @@
         <v>56</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E29">
         <v>1</v>

</xml_diff>